<commit_message>
Header.js + Menu.js added
</commit_message>
<xml_diff>
--- a/LogBoek.xlsx
+++ b/LogBoek.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>DATUM</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Gulp Test</t>
+  </si>
+  <si>
+    <t>aanmaken basis uitzicht (componetns, header + menu)</t>
   </si>
 </sst>
 </file>
@@ -535,8 +538,8 @@
   </sheetPr>
   <dimension ref="B1:C8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -593,8 +596,12 @@
       </c>
     </row>
     <row r="7" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="5">
+        <v>43151</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
@@ -620,6 +627,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA3F7D94069FF64A86F7DFF56D60E3BE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c32302c77d4085ecf495bdddb7f5e889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4f35948-e619-41b3-aa29-22878b09cfd2" xmlns:ns3="40262f94-9f35-4ac3-9a90-690165a166b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ab5ae46be95f9d0be6107e8200be7a2" ns2:_="" ns3:_="">
     <xsd:import namespace="a4f35948-e619-41b3-aa29-22878b09cfd2"/>
@@ -800,27 +827,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B53890C6-895E-4346-BCB4-738C50EDC5D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -837,22 +862,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Menu & Logo plaats toegevoegd
</commit_message>
<xml_diff>
--- a/LogBoek.xlsx
+++ b/LogBoek.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>DATUM</t>
   </si>
@@ -46,7 +46,10 @@
     <t>Gulp Test</t>
   </si>
   <si>
-    <t>aanmaken basis uitzicht (componetns, header + menu)</t>
+    <t>aanmaken header</t>
+  </si>
+  <si>
+    <t>aanmaken menu + logo plaats</t>
   </si>
 </sst>
 </file>
@@ -191,15 +194,12 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="4">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10">
       <alignment vertical="center"/>
@@ -539,7 +539,7 @@
   <dimension ref="B1:C8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -550,62 +550,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" s="1" customFormat="1" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1"/>
     </row>
     <row r="2" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>43150</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>43151</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>43151</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>43151</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>43151</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="4">
+        <v>43152</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations xWindow="45" yWindow="267" count="4">
@@ -627,26 +631,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA3F7D94069FF64A86F7DFF56D60E3BE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c32302c77d4085ecf495bdddb7f5e889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4f35948-e619-41b3-aa29-22878b09cfd2" xmlns:ns3="40262f94-9f35-4ac3-9a90-690165a166b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ab5ae46be95f9d0be6107e8200be7a2" ns2:_="" ns3:_="">
     <xsd:import namespace="a4f35948-e619-41b3-aa29-22878b09cfd2"/>
@@ -827,25 +811,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B53890C6-895E-4346-BCB4-738C50EDC5D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -862,4 +848,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>